<commit_message>
plotted toy-spam with min 5
</commit_message>
<xml_diff>
--- a/results/mp/tinybert/toy-spam/confidence/126/stop-words-0.1/avg_0.002_scores.xlsx
+++ b/results/mp/tinybert/toy-spam/confidence/126/stop-words-0.1/avg_0.002_scores.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="110">
   <si>
     <t>anchor score</t>
   </si>
@@ -40,216 +40,204 @@
     <t>name</t>
   </si>
   <si>
+    <t>garbage</t>
+  </si>
+  <si>
     <t>poorly</t>
   </si>
   <si>
     <t>disappointing</t>
   </si>
   <si>
+    <t>crap</t>
+  </si>
+  <si>
+    <t>thin</t>
+  </si>
+  <si>
+    <t>broke</t>
+  </si>
+  <si>
+    <t>ripped</t>
+  </si>
+  <si>
     <t>however</t>
   </si>
   <si>
+    <t>disappointed</t>
+  </si>
+  <si>
+    <t>poor</t>
+  </si>
+  <si>
     <t>disappointment</t>
   </si>
   <si>
-    <t>bottom</t>
-  </si>
-  <si>
-    <t>thin</t>
-  </si>
-  <si>
-    <t>ripped</t>
-  </si>
-  <si>
     <t>returned</t>
   </si>
   <si>
-    <t>crap</t>
-  </si>
-  <si>
-    <t>poor</t>
-  </si>
-  <si>
-    <t>disappointed</t>
-  </si>
-  <si>
-    <t>broke</t>
-  </si>
-  <si>
-    <t>stopped</t>
+    <t>inches</t>
+  </si>
+  <si>
+    <t>waste</t>
+  </si>
+  <si>
+    <t>smaller</t>
+  </si>
+  <si>
+    <t>instead</t>
   </si>
   <si>
     <t>worst</t>
   </si>
   <si>
-    <t>waste</t>
-  </si>
-  <si>
-    <t>smaller</t>
+    <t>probably</t>
+  </si>
+  <si>
+    <t>tiny</t>
+  </si>
+  <si>
+    <t>junk</t>
+  </si>
+  <si>
+    <t>water</t>
   </si>
   <si>
     <t>pool</t>
   </si>
   <si>
-    <t>water</t>
-  </si>
-  <si>
-    <t>junk</t>
-  </si>
-  <si>
-    <t>instead</t>
-  </si>
-  <si>
-    <t>probably</t>
+    <t>broken</t>
   </si>
   <si>
     <t>guess</t>
   </si>
   <si>
+    <t>small</t>
+  </si>
+  <si>
+    <t>okay</t>
+  </si>
+  <si>
     <t>missing</t>
   </si>
   <si>
-    <t>tiny</t>
-  </si>
-  <si>
-    <t>low</t>
-  </si>
-  <si>
-    <t>small</t>
-  </si>
-  <si>
-    <t>okay</t>
+    <t>un</t>
+  </si>
+  <si>
+    <t>less</t>
+  </si>
+  <si>
+    <t>lasted</t>
+  </si>
+  <si>
+    <t>paint</t>
+  </si>
+  <si>
+    <t>plastic</t>
+  </si>
+  <si>
+    <t>apart</t>
   </si>
   <si>
     <t>short</t>
   </si>
   <si>
-    <t>paint</t>
+    <t>di</t>
+  </si>
+  <si>
+    <t>ok</t>
   </si>
   <si>
     <t>tried</t>
   </si>
   <si>
-    <t>plastic</t>
-  </si>
-  <si>
-    <t>lasted</t>
-  </si>
-  <si>
-    <t>un</t>
-  </si>
-  <si>
-    <t>apart</t>
-  </si>
-  <si>
-    <t>broken</t>
-  </si>
-  <si>
-    <t>less</t>
-  </si>
-  <si>
-    <t>di</t>
-  </si>
-  <si>
-    <t>seem</t>
+    <t>fell</t>
+  </si>
+  <si>
+    <t>fl</t>
+  </si>
+  <si>
+    <t>thought</t>
+  </si>
+  <si>
+    <t>difficult</t>
+  </si>
+  <si>
+    <t>pay</t>
+  </si>
+  <si>
+    <t>cheap</t>
+  </si>
+  <si>
+    <t>half</t>
   </si>
   <si>
     <t>maybe</t>
   </si>
   <si>
-    <t>cheap</t>
-  </si>
-  <si>
-    <t>fell</t>
-  </si>
-  <si>
-    <t>thought</t>
-  </si>
-  <si>
-    <t>ok</t>
-  </si>
-  <si>
-    <t>difficult</t>
-  </si>
-  <si>
-    <t>half</t>
-  </si>
-  <si>
-    <t>light</t>
+    <t>bit</t>
   </si>
   <si>
     <t>though</t>
   </si>
   <si>
-    <t>fl</t>
-  </si>
-  <si>
-    <t>pay</t>
-  </si>
-  <si>
     <t>bad</t>
   </si>
   <si>
-    <t>bit</t>
-  </si>
-  <si>
-    <t>sound</t>
-  </si>
-  <si>
     <t>size</t>
   </si>
   <si>
+    <t>minutes</t>
+  </si>
+  <si>
+    <t>nothing</t>
+  </si>
+  <si>
+    <t>used</t>
+  </si>
+  <si>
+    <t>hard</t>
+  </si>
+  <si>
+    <t>item</t>
+  </si>
+  <si>
+    <t>would</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
     <t>picture</t>
   </si>
   <si>
-    <t>minutes</t>
-  </si>
-  <si>
-    <t>color</t>
-  </si>
-  <si>
-    <t>1</t>
-  </si>
-  <si>
-    <t>hard</t>
+    <t>back</t>
+  </si>
+  <si>
+    <t>worked</t>
+  </si>
+  <si>
+    <t>could</t>
   </si>
   <si>
     <t>money</t>
   </si>
   <si>
-    <t>item</t>
-  </si>
-  <si>
-    <t>would</t>
-  </si>
-  <si>
     <t>work</t>
   </si>
   <si>
-    <t>back</t>
-  </si>
-  <si>
     <t>better</t>
   </si>
   <si>
-    <t>worked</t>
+    <t>product</t>
   </si>
   <si>
     <t>price</t>
   </si>
   <si>
-    <t>used</t>
-  </si>
-  <si>
     <t>need</t>
   </si>
   <si>
-    <t>could</t>
-  </si>
-  <si>
-    <t>product</t>
-  </si>
-  <si>
     <t>3</t>
   </si>
   <si>
@@ -259,28 +247,34 @@
     <t>pieces</t>
   </si>
   <si>
+    <t>put</t>
+  </si>
+  <si>
+    <t>box</t>
+  </si>
+  <si>
+    <t>expected</t>
+  </si>
+  <si>
     <t>2</t>
   </si>
   <si>
-    <t>expected</t>
+    <t>5</t>
+  </si>
+  <si>
+    <t>buy</t>
+  </si>
+  <si>
+    <t>like</t>
   </si>
   <si>
     <t>even</t>
   </si>
   <si>
-    <t>like</t>
-  </si>
-  <si>
     <t>little</t>
   </si>
   <si>
-    <t>made</t>
-  </si>
-  <si>
-    <t>buy</t>
-  </si>
-  <si>
-    <t>get</t>
+    <t>much</t>
   </si>
   <si>
     <t>one</t>
@@ -292,21 +286,18 @@
     <t>negative</t>
   </si>
   <si>
+    <t>awesome</t>
+  </si>
+  <si>
     <t>wonderful</t>
   </si>
   <si>
-    <t>awesome</t>
-  </si>
-  <si>
     <t>amazing</t>
   </si>
   <si>
     <t>favorite</t>
   </si>
   <si>
-    <t>enjoyable</t>
-  </si>
-  <si>
     <t>classic</t>
   </si>
   <si>
@@ -337,16 +328,16 @@
     <t>friends</t>
   </si>
   <si>
+    <t>learn</t>
+  </si>
+  <si>
     <t>christmas</t>
   </si>
   <si>
+    <t>fun</t>
+  </si>
+  <si>
     <t>enjoy</t>
-  </si>
-  <si>
-    <t>fun</t>
-  </si>
-  <si>
-    <t>family</t>
   </si>
   <si>
     <t>game</t>
@@ -710,7 +701,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q85"/>
+  <dimension ref="A1:Q83"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -718,10 +709,10 @@
   <sheetData>
     <row r="1" spans="1:17">
       <c r="A1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="J1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
     </row>
     <row r="2" spans="1:17">
@@ -779,13 +770,13 @@
         <v>8</v>
       </c>
       <c r="B3">
-        <v>0.9782608695652174</v>
+        <v>1</v>
       </c>
       <c r="C3">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="D3">
-        <v>45</v>
+        <v>17</v>
       </c>
       <c r="E3">
         <v>0</v>
@@ -797,19 +788,19 @@
         <v>0</v>
       </c>
       <c r="H3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="J3" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="K3">
-        <v>0.8392857142857143</v>
+        <v>0.8461538461538461</v>
       </c>
       <c r="L3">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="M3">
-        <v>47</v>
+        <v>55</v>
       </c>
       <c r="N3">
         <v>1</v>
@@ -821,7 +812,7 @@
         <v>0</v>
       </c>
       <c r="Q3">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:17">
@@ -829,13 +820,13 @@
         <v>9</v>
       </c>
       <c r="B4">
-        <v>0.8409090909090909</v>
+        <v>0.9782608695652174</v>
       </c>
       <c r="C4">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="D4">
-        <v>37</v>
+        <v>45</v>
       </c>
       <c r="E4">
         <v>0</v>
@@ -847,19 +838,19 @@
         <v>0</v>
       </c>
       <c r="H4">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="J4" s="1" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="K4">
-        <v>0.8307692307692308</v>
+        <v>0.8214285714285714</v>
       </c>
       <c r="L4">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="M4">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="N4">
         <v>1</v>
@@ -871,7 +862,7 @@
         <v>0</v>
       </c>
       <c r="Q4">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:17">
@@ -879,13 +870,13 @@
         <v>10</v>
       </c>
       <c r="B5">
-        <v>0.8125</v>
+        <v>0.8636363636363636</v>
       </c>
       <c r="C5">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="D5">
-        <v>52</v>
+        <v>38</v>
       </c>
       <c r="E5">
         <v>0</v>
@@ -897,10 +888,10 @@
         <v>0</v>
       </c>
       <c r="H5">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="J5" s="1" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="K5">
         <v>0.7777777777777778</v>
@@ -950,16 +941,16 @@
         <v>4</v>
       </c>
       <c r="J6" s="1" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="K6">
-        <v>0.7096774193548387</v>
+        <v>0.6881720430107527</v>
       </c>
       <c r="L6">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="M6">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="N6">
         <v>1</v>
@@ -971,7 +962,7 @@
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>27</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:17">
@@ -979,13 +970,13 @@
         <v>12</v>
       </c>
       <c r="B7">
-        <v>0.8</v>
+        <v>0.7931034482758621</v>
       </c>
       <c r="C7">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="D7">
-        <v>16</v>
+        <v>23</v>
       </c>
       <c r="E7">
         <v>0</v>
@@ -997,19 +988,19 @@
         <v>0</v>
       </c>
       <c r="H7">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="J7" s="1" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="K7">
-        <v>0.625</v>
+        <v>0.6415094339622641</v>
       </c>
       <c r="L7">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="M7">
-        <v>15</v>
+        <v>34</v>
       </c>
       <c r="N7">
         <v>1</v>
@@ -1021,7 +1012,7 @@
         <v>0</v>
       </c>
       <c r="Q7">
-        <v>9</v>
+        <v>19</v>
       </c>
     </row>
     <row r="8" spans="1:17">
@@ -1029,13 +1020,13 @@
         <v>13</v>
       </c>
       <c r="B8">
-        <v>0.7931034482758621</v>
+        <v>0.7815533980582524</v>
       </c>
       <c r="C8">
-        <v>23</v>
+        <v>161</v>
       </c>
       <c r="D8">
-        <v>23</v>
+        <v>161</v>
       </c>
       <c r="E8">
         <v>0</v>
@@ -1047,19 +1038,19 @@
         <v>0</v>
       </c>
       <c r="H8">
-        <v>6</v>
+        <v>45</v>
       </c>
       <c r="J8" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="K8">
-        <v>0.5471698113207547</v>
+        <v>0.5</v>
       </c>
       <c r="L8">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="M8">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="N8">
         <v>1</v>
@@ -1071,7 +1062,7 @@
         <v>0</v>
       </c>
       <c r="Q8">
-        <v>24</v>
+        <v>32</v>
       </c>
     </row>
     <row r="9" spans="1:17">
@@ -1100,16 +1091,16 @@
         <v>6</v>
       </c>
       <c r="J9" s="1" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="K9">
-        <v>0.53125</v>
+        <v>0.463768115942029</v>
       </c>
       <c r="L9">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="M9">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="N9">
         <v>1</v>
@@ -1121,7 +1112,7 @@
         <v>0</v>
       </c>
       <c r="Q9">
-        <v>30</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="1:17">
@@ -1129,13 +1120,13 @@
         <v>15</v>
       </c>
       <c r="B10">
-        <v>0.7631578947368421</v>
+        <v>0.75</v>
       </c>
       <c r="C10">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="D10">
-        <v>29</v>
+        <v>48</v>
       </c>
       <c r="E10">
         <v>0</v>
@@ -1147,19 +1138,19 @@
         <v>0</v>
       </c>
       <c r="H10">
-        <v>9</v>
+        <v>16</v>
       </c>
       <c r="J10" s="1" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="K10">
-        <v>0.391304347826087</v>
+        <v>0.3360655737704918</v>
       </c>
       <c r="L10">
-        <v>27</v>
+        <v>410</v>
       </c>
       <c r="M10">
-        <v>27</v>
+        <v>410</v>
       </c>
       <c r="N10">
         <v>1</v>
@@ -1171,7 +1162,7 @@
         <v>0</v>
       </c>
       <c r="Q10">
-        <v>42</v>
+        <v>810</v>
       </c>
     </row>
     <row r="11" spans="1:17">
@@ -1179,13 +1170,13 @@
         <v>16</v>
       </c>
       <c r="B11">
-        <v>0.7619047619047619</v>
+        <v>0.7473118279569892</v>
       </c>
       <c r="C11">
-        <v>16</v>
+        <v>139</v>
       </c>
       <c r="D11">
-        <v>16</v>
+        <v>139</v>
       </c>
       <c r="E11">
         <v>0</v>
@@ -1197,19 +1188,19 @@
         <v>0</v>
       </c>
       <c r="H11">
-        <v>5</v>
+        <v>47</v>
       </c>
       <c r="J11" s="1" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="K11">
-        <v>0.3305988515176374</v>
+        <v>0.2926829268292683</v>
       </c>
       <c r="L11">
-        <v>403</v>
+        <v>204</v>
       </c>
       <c r="M11">
-        <v>404</v>
+        <v>204</v>
       </c>
       <c r="N11">
         <v>1</v>
@@ -1218,10 +1209,10 @@
         <v>0</v>
       </c>
       <c r="P11" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q11">
-        <v>816</v>
+        <v>493</v>
       </c>
     </row>
     <row r="12" spans="1:17">
@@ -1250,16 +1241,16 @@
         <v>19</v>
       </c>
       <c r="J12" s="1" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="K12">
-        <v>0.2826398852223816</v>
+        <v>0.2593360995850623</v>
       </c>
       <c r="L12">
-        <v>197</v>
+        <v>125</v>
       </c>
       <c r="M12">
-        <v>197</v>
+        <v>125</v>
       </c>
       <c r="N12">
         <v>1</v>
@@ -1271,7 +1262,7 @@
         <v>0</v>
       </c>
       <c r="Q12">
-        <v>500</v>
+        <v>357</v>
       </c>
     </row>
     <row r="13" spans="1:17">
@@ -1279,13 +1270,13 @@
         <v>18</v>
       </c>
       <c r="B13">
-        <v>0.7204301075268817</v>
+        <v>0.7142857142857143</v>
       </c>
       <c r="C13">
-        <v>134</v>
+        <v>15</v>
       </c>
       <c r="D13">
-        <v>134</v>
+        <v>15</v>
       </c>
       <c r="E13">
         <v>0</v>
@@ -1297,19 +1288,19 @@
         <v>0</v>
       </c>
       <c r="H13">
-        <v>52</v>
+        <v>6</v>
       </c>
       <c r="J13" s="1" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="K13">
-        <v>0.2655601659751037</v>
+        <v>0.2583333333333334</v>
       </c>
       <c r="L13">
-        <v>128</v>
+        <v>31</v>
       </c>
       <c r="M13">
-        <v>128</v>
+        <v>31</v>
       </c>
       <c r="N13">
         <v>1</v>
@@ -1321,7 +1312,7 @@
         <v>0</v>
       </c>
       <c r="Q13">
-        <v>354</v>
+        <v>89</v>
       </c>
     </row>
     <row r="14" spans="1:17">
@@ -1329,13 +1320,13 @@
         <v>19</v>
       </c>
       <c r="B14">
-        <v>0.6990291262135923</v>
+        <v>0.6842105263157895</v>
       </c>
       <c r="C14">
-        <v>144</v>
+        <v>26</v>
       </c>
       <c r="D14">
-        <v>144</v>
+        <v>26</v>
       </c>
       <c r="E14">
         <v>0</v>
@@ -1347,19 +1338,19 @@
         <v>0</v>
       </c>
       <c r="H14">
-        <v>62</v>
+        <v>12</v>
       </c>
       <c r="J14" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="K14">
-        <v>0.2583333333333334</v>
+        <v>0.1987951807228916</v>
       </c>
       <c r="L14">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="M14">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="N14">
         <v>1</v>
@@ -1371,7 +1362,7 @@
         <v>0</v>
       </c>
       <c r="Q14">
-        <v>89</v>
+        <v>133</v>
       </c>
     </row>
     <row r="15" spans="1:17">
@@ -1400,16 +1391,16 @@
         <v>7</v>
       </c>
       <c r="J15" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="K15">
-        <v>0.2108433734939759</v>
+        <v>0.1773700305810398</v>
       </c>
       <c r="L15">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="M15">
-        <v>35</v>
+        <v>58</v>
       </c>
       <c r="N15">
         <v>1</v>
@@ -1421,7 +1412,7 @@
         <v>0</v>
       </c>
       <c r="Q15">
-        <v>131</v>
+        <v>269</v>
       </c>
     </row>
     <row r="16" spans="1:17">
@@ -1429,13 +1420,13 @@
         <v>21</v>
       </c>
       <c r="B16">
-        <v>0.68</v>
+        <v>0.6756756756756757</v>
       </c>
       <c r="C16">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="D16">
-        <v>17</v>
+        <v>100</v>
       </c>
       <c r="E16">
         <v>0</v>
@@ -1447,19 +1438,19 @@
         <v>0</v>
       </c>
       <c r="H16">
-        <v>8</v>
+        <v>48</v>
       </c>
       <c r="J16" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="K16">
-        <v>0.1865443425076453</v>
+        <v>0.1375661375661376</v>
       </c>
       <c r="L16">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="M16">
-        <v>61</v>
+        <v>26</v>
       </c>
       <c r="N16">
         <v>1</v>
@@ -1471,7 +1462,7 @@
         <v>0</v>
       </c>
       <c r="Q16">
-        <v>266</v>
+        <v>163</v>
       </c>
     </row>
     <row r="17" spans="1:17">
@@ -1479,13 +1470,13 @@
         <v>22</v>
       </c>
       <c r="B17">
-        <v>0.6621621621621622</v>
+        <v>0.6050420168067226</v>
       </c>
       <c r="C17">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="D17">
-        <v>98</v>
+        <v>72</v>
       </c>
       <c r="E17">
         <v>0</v>
@@ -1497,19 +1488,19 @@
         <v>0</v>
       </c>
       <c r="H17">
-        <v>50</v>
+        <v>47</v>
       </c>
       <c r="J17" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="K17">
-        <v>0.1375661375661376</v>
+        <v>0.125</v>
       </c>
       <c r="L17">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="M17">
-        <v>26</v>
+        <v>16</v>
       </c>
       <c r="N17">
         <v>1</v>
@@ -1521,7 +1512,7 @@
         <v>0</v>
       </c>
       <c r="Q17">
-        <v>163</v>
+        <v>112</v>
       </c>
     </row>
     <row r="18" spans="1:17">
@@ -1529,13 +1520,13 @@
         <v>23</v>
       </c>
       <c r="B18">
-        <v>0.6134453781512605</v>
+        <v>0.6041666666666666</v>
       </c>
       <c r="C18">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="D18">
-        <v>73</v>
+        <v>29</v>
       </c>
       <c r="E18">
         <v>0</v>
@@ -1547,19 +1538,19 @@
         <v>0</v>
       </c>
       <c r="H18">
-        <v>46</v>
+        <v>19</v>
       </c>
       <c r="J18" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="K18">
-        <v>0.108433734939759</v>
+        <v>0.08433734939759036</v>
       </c>
       <c r="L18">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="M18">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="N18">
         <v>1</v>
@@ -1571,7 +1562,7 @@
         <v>0</v>
       </c>
       <c r="Q18">
-        <v>222</v>
+        <v>228</v>
       </c>
     </row>
     <row r="19" spans="1:17">
@@ -1582,10 +1573,10 @@
         <v>0.6</v>
       </c>
       <c r="C19">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="D19">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="E19">
         <v>0</v>
@@ -1597,19 +1588,19 @@
         <v>0</v>
       </c>
       <c r="H19">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="J19" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="K19">
-        <v>0.09139784946236559</v>
+        <v>0.08326029798422437</v>
       </c>
       <c r="L19">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="M19">
-        <v>17</v>
+        <v>95</v>
       </c>
       <c r="N19">
         <v>1</v>
@@ -1621,7 +1612,7 @@
         <v>0</v>
       </c>
       <c r="Q19">
-        <v>169</v>
+        <v>1046</v>
       </c>
     </row>
     <row r="20" spans="1:17">
@@ -1629,13 +1620,13 @@
         <v>25</v>
       </c>
       <c r="B20">
-        <v>0.5952380952380952</v>
+        <v>0.5789473684210527</v>
       </c>
       <c r="C20">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="D20">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="E20">
         <v>0</v>
@@ -1647,31 +1638,31 @@
         <v>0</v>
       </c>
       <c r="H20">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="J20" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="K20">
-        <v>0.07280701754385965</v>
+        <v>0.08064516129032258</v>
       </c>
       <c r="L20">
-        <v>83</v>
+        <v>15</v>
       </c>
       <c r="M20">
-        <v>84</v>
+        <v>15</v>
       </c>
       <c r="N20">
-        <v>0.99</v>
+        <v>1</v>
       </c>
       <c r="O20">
-        <v>0.01000000000000001</v>
+        <v>0</v>
       </c>
       <c r="P20" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="Q20">
-        <v>1057</v>
+        <v>171</v>
       </c>
     </row>
     <row r="21" spans="1:17">
@@ -1679,13 +1670,13 @@
         <v>26</v>
       </c>
       <c r="B21">
-        <v>0.5818181818181818</v>
+        <v>0.5428571428571428</v>
       </c>
       <c r="C21">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="D21">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="E21">
         <v>0</v>
@@ -1697,31 +1688,31 @@
         <v>0</v>
       </c>
       <c r="H21">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="J21" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="K21">
-        <v>0.04735376044568245</v>
+        <v>0.03636363636363636</v>
       </c>
       <c r="L21">
-        <v>17</v>
+        <v>56</v>
       </c>
       <c r="M21">
-        <v>17</v>
+        <v>57</v>
       </c>
       <c r="N21">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="O21">
-        <v>0</v>
+        <v>0.02000000000000002</v>
       </c>
       <c r="P21" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="Q21">
-        <v>342</v>
+        <v>1484</v>
       </c>
     </row>
     <row r="22" spans="1:17">
@@ -1729,13 +1720,13 @@
         <v>27</v>
       </c>
       <c r="B22">
-        <v>0.5208333333333334</v>
+        <v>0.5272727272727272</v>
       </c>
       <c r="C22">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="D22">
-        <v>25</v>
+        <v>29</v>
       </c>
       <c r="E22">
         <v>0</v>
@@ -1747,31 +1738,7 @@
         <v>0</v>
       </c>
       <c r="H22">
-        <v>23</v>
-      </c>
-      <c r="J22" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="K22">
-        <v>0.03378817413905133</v>
-      </c>
-      <c r="L22">
-        <v>52</v>
-      </c>
-      <c r="M22">
-        <v>54</v>
-      </c>
-      <c r="N22">
-        <v>0.96</v>
-      </c>
-      <c r="O22">
-        <v>0.04000000000000004</v>
-      </c>
-      <c r="P22" t="b">
-        <v>1</v>
-      </c>
-      <c r="Q22">
-        <v>1487</v>
+        <v>26</v>
       </c>
     </row>
     <row r="23" spans="1:17">
@@ -1779,13 +1746,13 @@
         <v>28</v>
       </c>
       <c r="B23">
-        <v>0.5</v>
+        <v>0.5238095238095238</v>
       </c>
       <c r="C23">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="D23">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="E23">
         <v>0</v>
@@ -1797,7 +1764,7 @@
         <v>0</v>
       </c>
       <c r="H23">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="24" spans="1:17">
@@ -1805,13 +1772,13 @@
         <v>29</v>
       </c>
       <c r="B24">
-        <v>0.5</v>
+        <v>0.5142857142857142</v>
       </c>
       <c r="C24">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="D24">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="E24">
         <v>0</v>
@@ -1823,7 +1790,7 @@
         <v>0</v>
       </c>
       <c r="H24">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="25" spans="1:17">
@@ -1831,13 +1798,13 @@
         <v>30</v>
       </c>
       <c r="B25">
-        <v>0.4888888888888889</v>
+        <v>0.5060240963855421</v>
       </c>
       <c r="C25">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="D25">
-        <v>22</v>
+        <v>42</v>
       </c>
       <c r="E25">
         <v>0</v>
@@ -1849,7 +1816,7 @@
         <v>0</v>
       </c>
       <c r="H25">
-        <v>23</v>
+        <v>41</v>
       </c>
     </row>
     <row r="26" spans="1:17">
@@ -1857,13 +1824,13 @@
         <v>31</v>
       </c>
       <c r="B26">
-        <v>0.4857142857142857</v>
+        <v>0.5</v>
       </c>
       <c r="C26">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="D26">
-        <v>17</v>
+        <v>27</v>
       </c>
       <c r="E26">
         <v>0</v>
@@ -1875,7 +1842,7 @@
         <v>0</v>
       </c>
       <c r="H26">
-        <v>18</v>
+        <v>27</v>
       </c>
     </row>
     <row r="27" spans="1:17">
@@ -1883,13 +1850,13 @@
         <v>32</v>
       </c>
       <c r="B27">
-        <v>0.4838709677419355</v>
+        <v>0.4985507246376812</v>
       </c>
       <c r="C27">
-        <v>15</v>
+        <v>172</v>
       </c>
       <c r="D27">
-        <v>15</v>
+        <v>172</v>
       </c>
       <c r="E27">
         <v>0</v>
@@ -1901,7 +1868,7 @@
         <v>0</v>
       </c>
       <c r="H27">
-        <v>16</v>
+        <v>173</v>
       </c>
     </row>
     <row r="28" spans="1:17">
@@ -1909,13 +1876,13 @@
         <v>33</v>
       </c>
       <c r="B28">
-        <v>0.4753623188405797</v>
+        <v>0.4814814814814815</v>
       </c>
       <c r="C28">
-        <v>164</v>
+        <v>26</v>
       </c>
       <c r="D28">
-        <v>164</v>
+        <v>26</v>
       </c>
       <c r="E28">
         <v>0</v>
@@ -1927,7 +1894,7 @@
         <v>0</v>
       </c>
       <c r="H28">
-        <v>181</v>
+        <v>28</v>
       </c>
     </row>
     <row r="29" spans="1:17">
@@ -1935,13 +1902,13 @@
         <v>34</v>
       </c>
       <c r="B29">
-        <v>0.462962962962963</v>
+        <v>0.4666666666666667</v>
       </c>
       <c r="C29">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D29">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="E29">
         <v>0</v>
@@ -1953,7 +1920,7 @@
         <v>0</v>
       </c>
       <c r="H29">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="30" spans="1:17">
@@ -1961,13 +1928,13 @@
         <v>35</v>
       </c>
       <c r="B30">
-        <v>0.4489795918367347</v>
+        <v>0.4418604651162791</v>
       </c>
       <c r="C30">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D30">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="E30">
         <v>0</v>
@@ -1979,7 +1946,7 @@
         <v>0</v>
       </c>
       <c r="H30">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:17">
@@ -1987,7 +1954,7 @@
         <v>36</v>
       </c>
       <c r="B31">
-        <v>0.4126984126984127</v>
+        <v>0.4333333333333333</v>
       </c>
       <c r="C31">
         <v>26</v>
@@ -2005,7 +1972,7 @@
         <v>0</v>
       </c>
       <c r="H31">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:17">
@@ -2013,13 +1980,13 @@
         <v>37</v>
       </c>
       <c r="B32">
-        <v>0.4098360655737705</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="C32">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="D32">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="E32">
         <v>0</v>
@@ -2031,7 +1998,7 @@
         <v>0</v>
       </c>
       <c r="H32">
-        <v>36</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:8">
@@ -2039,13 +2006,13 @@
         <v>38</v>
       </c>
       <c r="B33">
-        <v>0.4094488188976378</v>
+        <v>0.4285714285714285</v>
       </c>
       <c r="C33">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="D33">
-        <v>52</v>
+        <v>27</v>
       </c>
       <c r="E33">
         <v>0</v>
@@ -2057,7 +2024,7 @@
         <v>0</v>
       </c>
       <c r="H33">
-        <v>75</v>
+        <v>36</v>
       </c>
     </row>
     <row r="34" spans="1:8">
@@ -2065,13 +2032,13 @@
         <v>39</v>
       </c>
       <c r="B34">
-        <v>0.4047619047619048</v>
+        <v>0.4251968503937008</v>
       </c>
       <c r="C34">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="D34">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="E34">
         <v>0</v>
@@ -2083,7 +2050,7 @@
         <v>0</v>
       </c>
       <c r="H34">
-        <v>25</v>
+        <v>73</v>
       </c>
     </row>
     <row r="35" spans="1:8">
@@ -2091,13 +2058,13 @@
         <v>40</v>
       </c>
       <c r="B35">
-        <v>0.3953488372093023</v>
+        <v>0.4210526315789473</v>
       </c>
       <c r="C35">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="D35">
-        <v>17</v>
+        <v>40</v>
       </c>
       <c r="E35">
         <v>0</v>
@@ -2109,7 +2076,7 @@
         <v>0</v>
       </c>
       <c r="H35">
-        <v>26</v>
+        <v>55</v>
       </c>
     </row>
     <row r="36" spans="1:8">
@@ -2117,13 +2084,13 @@
         <v>41</v>
       </c>
       <c r="B36">
-        <v>0.3894736842105263</v>
+        <v>0.3877551020408163</v>
       </c>
       <c r="C36">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="D36">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="E36">
         <v>0</v>
@@ -2135,7 +2102,7 @@
         <v>0</v>
       </c>
       <c r="H36">
-        <v>58</v>
+        <v>30</v>
       </c>
     </row>
     <row r="37" spans="1:8">
@@ -2143,13 +2110,13 @@
         <v>42</v>
       </c>
       <c r="B37">
-        <v>0.3855421686746988</v>
+        <v>0.375</v>
       </c>
       <c r="C37">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="D37">
-        <v>32</v>
+        <v>24</v>
       </c>
       <c r="E37">
         <v>0</v>
@@ -2161,7 +2128,7 @@
         <v>0</v>
       </c>
       <c r="H37">
-        <v>51</v>
+        <v>40</v>
       </c>
     </row>
     <row r="38" spans="1:8">
@@ -2169,13 +2136,13 @@
         <v>43</v>
       </c>
       <c r="B38">
-        <v>0.3833333333333334</v>
+        <v>0.34375</v>
       </c>
       <c r="C38">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="D38">
-        <v>23</v>
+        <v>44</v>
       </c>
       <c r="E38">
         <v>0</v>
@@ -2187,7 +2154,7 @@
         <v>0</v>
       </c>
       <c r="H38">
-        <v>37</v>
+        <v>84</v>
       </c>
     </row>
     <row r="39" spans="1:8">
@@ -2195,13 +2162,13 @@
         <v>44</v>
       </c>
       <c r="B39">
-        <v>0.359375</v>
+        <v>0.3278688524590164</v>
       </c>
       <c r="C39">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="D39">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="E39">
         <v>0</v>
@@ -2221,13 +2188,13 @@
         <v>45</v>
       </c>
       <c r="B40">
-        <v>0.3061224489795918</v>
+        <v>0.3272727272727273</v>
       </c>
       <c r="C40">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="D40">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="E40">
         <v>0</v>
@@ -2239,7 +2206,7 @@
         <v>0</v>
       </c>
       <c r="H40">
-        <v>34</v>
+        <v>37</v>
       </c>
     </row>
     <row r="41" spans="1:8">
@@ -2247,13 +2214,13 @@
         <v>46</v>
       </c>
       <c r="B41">
-        <v>0.3035714285714285</v>
+        <v>0.3103448275862069</v>
       </c>
       <c r="C41">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D41">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E41">
         <v>0</v>
@@ -2265,7 +2232,7 @@
         <v>0</v>
       </c>
       <c r="H41">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:8">
@@ -2273,13 +2240,13 @@
         <v>47</v>
       </c>
       <c r="B42">
-        <v>0.2985781990521327</v>
+        <v>0.3069306930693069</v>
       </c>
       <c r="C42">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D42">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E42">
         <v>0</v>
@@ -2291,7 +2258,7 @@
         <v>0</v>
       </c>
       <c r="H42">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="43" spans="1:8">
@@ -2299,13 +2266,13 @@
         <v>48</v>
       </c>
       <c r="B43">
-        <v>0.2909090909090909</v>
+        <v>0.303370786516854</v>
       </c>
       <c r="C43">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="D43">
-        <v>16</v>
+        <v>27</v>
       </c>
       <c r="E43">
         <v>0</v>
@@ -2317,7 +2284,7 @@
         <v>0</v>
       </c>
       <c r="H43">
-        <v>39</v>
+        <v>62</v>
       </c>
     </row>
     <row r="44" spans="1:8">
@@ -2325,13 +2292,13 @@
         <v>49</v>
       </c>
       <c r="B44">
-        <v>0.2871287128712871</v>
+        <v>0.3015873015873016</v>
       </c>
       <c r="C44">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="D44">
-        <v>58</v>
+        <v>19</v>
       </c>
       <c r="E44">
         <v>0</v>
@@ -2343,7 +2310,7 @@
         <v>0</v>
       </c>
       <c r="H44">
-        <v>144</v>
+        <v>44</v>
       </c>
     </row>
     <row r="45" spans="1:8">
@@ -2351,13 +2318,13 @@
         <v>50</v>
       </c>
       <c r="B45">
-        <v>0.28125</v>
+        <v>0.2890995260663507</v>
       </c>
       <c r="C45">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="D45">
-        <v>36</v>
+        <v>61</v>
       </c>
       <c r="E45">
         <v>0</v>
@@ -2369,7 +2336,7 @@
         <v>0</v>
       </c>
       <c r="H45">
-        <v>92</v>
+        <v>150</v>
       </c>
     </row>
     <row r="46" spans="1:8">
@@ -2377,13 +2344,13 @@
         <v>51</v>
       </c>
       <c r="B46">
-        <v>0.2808988764044944</v>
+        <v>0.2777777777777778</v>
       </c>
       <c r="C46">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="D46">
-        <v>25</v>
+        <v>15</v>
       </c>
       <c r="E46">
         <v>0</v>
@@ -2395,7 +2362,7 @@
         <v>0</v>
       </c>
       <c r="H46">
-        <v>64</v>
+        <v>39</v>
       </c>
     </row>
     <row r="47" spans="1:8">
@@ -2403,7 +2370,7 @@
         <v>52</v>
       </c>
       <c r="B47">
-        <v>0.2777777777777778</v>
+        <v>0.2678571428571428</v>
       </c>
       <c r="C47">
         <v>15</v>
@@ -2421,7 +2388,7 @@
         <v>0</v>
       </c>
       <c r="H47">
-        <v>39</v>
+        <v>41</v>
       </c>
     </row>
     <row r="48" spans="1:8">
@@ -2429,13 +2396,13 @@
         <v>53</v>
       </c>
       <c r="B48">
-        <v>0.2678571428571428</v>
+        <v>0.2653061224489796</v>
       </c>
       <c r="C48">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="D48">
-        <v>15</v>
+        <v>26</v>
       </c>
       <c r="E48">
         <v>0</v>
@@ -2447,7 +2414,7 @@
         <v>0</v>
       </c>
       <c r="H48">
-        <v>41</v>
+        <v>72</v>
       </c>
     </row>
     <row r="49" spans="1:8">
@@ -2455,13 +2422,13 @@
         <v>54</v>
       </c>
       <c r="B49">
-        <v>0.264957264957265</v>
+        <v>0.2564102564102564</v>
       </c>
       <c r="C49">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D49">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="E49">
         <v>0</v>
@@ -2473,7 +2440,7 @@
         <v>0</v>
       </c>
       <c r="H49">
-        <v>86</v>
+        <v>87</v>
       </c>
     </row>
     <row r="50" spans="1:8">
@@ -2481,13 +2448,13 @@
         <v>55</v>
       </c>
       <c r="B50">
-        <v>0.2586206896551724</v>
+        <v>0.2388059701492537</v>
       </c>
       <c r="C50">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D50">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="E50">
         <v>0</v>
@@ -2499,7 +2466,7 @@
         <v>0</v>
       </c>
       <c r="H50">
-        <v>43</v>
+        <v>51</v>
       </c>
     </row>
     <row r="51" spans="1:8">
@@ -2507,13 +2474,13 @@
         <v>56</v>
       </c>
       <c r="B51">
-        <v>0.253968253968254</v>
+        <v>0.2164948453608248</v>
       </c>
       <c r="C51">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="D51">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="E51">
         <v>0</v>
@@ -2525,7 +2492,7 @@
         <v>0</v>
       </c>
       <c r="H51">
-        <v>47</v>
+        <v>152</v>
       </c>
     </row>
     <row r="52" spans="1:8">
@@ -2533,7 +2500,7 @@
         <v>57</v>
       </c>
       <c r="B52">
-        <v>0.2388059701492537</v>
+        <v>0.2162162162162162</v>
       </c>
       <c r="C52">
         <v>16</v>
@@ -2551,7 +2518,7 @@
         <v>0</v>
       </c>
       <c r="H52">
-        <v>51</v>
+        <v>58</v>
       </c>
     </row>
     <row r="53" spans="1:8">
@@ -2559,13 +2526,13 @@
         <v>58</v>
       </c>
       <c r="B53">
-        <v>0.2346938775510204</v>
+        <v>0.1978021978021978</v>
       </c>
       <c r="C53">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="D53">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="E53">
         <v>0</v>
@@ -2577,7 +2544,7 @@
         <v>0</v>
       </c>
       <c r="H53">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="54" spans="1:8">
@@ -2585,13 +2552,13 @@
         <v>59</v>
       </c>
       <c r="B54">
-        <v>0.2318840579710145</v>
+        <v>0.1942857142857143</v>
       </c>
       <c r="C54">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="D54">
-        <v>16</v>
+        <v>34</v>
       </c>
       <c r="E54">
         <v>0</v>
@@ -2603,7 +2570,7 @@
         <v>0</v>
       </c>
       <c r="H54">
-        <v>53</v>
+        <v>141</v>
       </c>
     </row>
     <row r="55" spans="1:8">
@@ -2611,13 +2578,13 @@
         <v>60</v>
       </c>
       <c r="B55">
-        <v>0.2164948453608248</v>
+        <v>0.185</v>
       </c>
       <c r="C55">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="D55">
-        <v>42</v>
+        <v>37</v>
       </c>
       <c r="E55">
         <v>0</v>
@@ -2629,7 +2596,7 @@
         <v>0</v>
       </c>
       <c r="H55">
-        <v>152</v>
+        <v>163</v>
       </c>
     </row>
     <row r="56" spans="1:8">
@@ -2637,13 +2604,13 @@
         <v>61</v>
       </c>
       <c r="B56">
-        <v>0.2164948453608248</v>
+        <v>0.1847826086956522</v>
       </c>
       <c r="C56">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="D56">
-        <v>21</v>
+        <v>51</v>
       </c>
       <c r="E56">
         <v>0</v>
@@ -2655,7 +2622,7 @@
         <v>0</v>
       </c>
       <c r="H56">
-        <v>76</v>
+        <v>225</v>
       </c>
     </row>
     <row r="57" spans="1:8">
@@ -2663,13 +2630,13 @@
         <v>62</v>
       </c>
       <c r="B57">
-        <v>0.2027027027027027</v>
+        <v>0.1795252225519288</v>
       </c>
       <c r="C57">
-        <v>15</v>
+        <v>121</v>
       </c>
       <c r="D57">
-        <v>15</v>
+        <v>121</v>
       </c>
       <c r="E57">
         <v>0</v>
@@ -2681,7 +2648,7 @@
         <v>0</v>
       </c>
       <c r="H57">
-        <v>59</v>
+        <v>553</v>
       </c>
     </row>
     <row r="58" spans="1:8">
@@ -2689,13 +2656,13 @@
         <v>63</v>
       </c>
       <c r="B58">
-        <v>0.2</v>
+        <v>0.1694915254237288</v>
       </c>
       <c r="C58">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="D58">
-        <v>15</v>
+        <v>20</v>
       </c>
       <c r="E58">
         <v>0</v>
@@ -2707,7 +2674,7 @@
         <v>0</v>
       </c>
       <c r="H58">
-        <v>60</v>
+        <v>98</v>
       </c>
     </row>
     <row r="59" spans="1:8">
@@ -2715,13 +2682,13 @@
         <v>64</v>
       </c>
       <c r="B59">
-        <v>0.1949152542372881</v>
+        <v>0.1649484536082474</v>
       </c>
       <c r="C59">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D59">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E59">
         <v>0</v>
@@ -2733,7 +2700,7 @@
         <v>0</v>
       </c>
       <c r="H59">
-        <v>95</v>
+        <v>81</v>
       </c>
     </row>
     <row r="60" spans="1:8">
@@ -2741,13 +2708,13 @@
         <v>65</v>
       </c>
       <c r="B60">
-        <v>0.185</v>
+        <v>0.1642857142857143</v>
       </c>
       <c r="C60">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="D60">
-        <v>37</v>
+        <v>23</v>
       </c>
       <c r="E60">
         <v>0</v>
@@ -2759,7 +2726,7 @@
         <v>0</v>
       </c>
       <c r="H60">
-        <v>163</v>
+        <v>117</v>
       </c>
     </row>
     <row r="61" spans="1:8">
@@ -2767,25 +2734,25 @@
         <v>66</v>
       </c>
       <c r="B61">
-        <v>0.1835443037974684</v>
+        <v>0.1588785046728972</v>
       </c>
       <c r="C61">
-        <v>58</v>
+        <v>17</v>
       </c>
       <c r="D61">
-        <v>58</v>
+        <v>18</v>
       </c>
       <c r="E61">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="F61">
-        <v>1</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="G61" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H61">
-        <v>258</v>
+        <v>90</v>
       </c>
     </row>
     <row r="62" spans="1:8">
@@ -2793,13 +2760,13 @@
         <v>67</v>
       </c>
       <c r="B62">
-        <v>0.1811594202898551</v>
+        <v>0.1528662420382166</v>
       </c>
       <c r="C62">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="D62">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="E62">
         <v>0</v>
@@ -2811,7 +2778,7 @@
         <v>0</v>
       </c>
       <c r="H62">
-        <v>226</v>
+        <v>133</v>
       </c>
     </row>
     <row r="63" spans="1:8">
@@ -2819,13 +2786,13 @@
         <v>68</v>
       </c>
       <c r="B63">
-        <v>0.172106824925816</v>
+        <v>0.1487341772151899</v>
       </c>
       <c r="C63">
-        <v>116</v>
+        <v>47</v>
       </c>
       <c r="D63">
-        <v>116</v>
+        <v>47</v>
       </c>
       <c r="E63">
         <v>0</v>
@@ -2837,7 +2804,7 @@
         <v>0</v>
       </c>
       <c r="H63">
-        <v>558</v>
+        <v>269</v>
       </c>
     </row>
     <row r="64" spans="1:8">
@@ -2845,13 +2812,13 @@
         <v>69</v>
       </c>
       <c r="B64">
-        <v>0.1677215189873418</v>
+        <v>0.1455696202531646</v>
       </c>
       <c r="C64">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="D64">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="E64">
         <v>0</v>
@@ -2863,7 +2830,7 @@
         <v>0</v>
       </c>
       <c r="H64">
-        <v>263</v>
+        <v>270</v>
       </c>
     </row>
     <row r="65" spans="1:8">
@@ -2871,13 +2838,13 @@
         <v>70</v>
       </c>
       <c r="B65">
-        <v>0.15</v>
+        <v>0.1355140186915888</v>
       </c>
       <c r="C65">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="D65">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="E65">
         <v>0</v>
@@ -2889,7 +2856,7 @@
         <v>0</v>
       </c>
       <c r="H65">
-        <v>119</v>
+        <v>185</v>
       </c>
     </row>
     <row r="66" spans="1:8">
@@ -2897,13 +2864,13 @@
         <v>71</v>
       </c>
       <c r="B66">
-        <v>0.1495327102803738</v>
+        <v>0.13215859030837</v>
       </c>
       <c r="C66">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="D66">
-        <v>32</v>
+        <v>60</v>
       </c>
       <c r="E66">
         <v>0</v>
@@ -2915,7 +2882,7 @@
         <v>0</v>
       </c>
       <c r="H66">
-        <v>182</v>
+        <v>394</v>
       </c>
     </row>
     <row r="67" spans="1:8">
@@ -2923,25 +2890,25 @@
         <v>72</v>
       </c>
       <c r="B67">
-        <v>0.1495327102803738</v>
+        <v>0.1235632183908046</v>
       </c>
       <c r="C67">
-        <v>16</v>
+        <v>43</v>
       </c>
       <c r="D67">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="E67">
-        <v>0.06</v>
+        <v>0</v>
       </c>
       <c r="F67">
-        <v>0.9399999999999999</v>
+        <v>1</v>
       </c>
       <c r="G67" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H67">
-        <v>91</v>
+        <v>305</v>
       </c>
     </row>
     <row r="68" spans="1:8">
@@ -2949,13 +2916,13 @@
         <v>73</v>
       </c>
       <c r="B68">
-        <v>0.1494252873563219</v>
+        <v>0.1230769230769231</v>
       </c>
       <c r="C68">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="D68">
-        <v>52</v>
+        <v>16</v>
       </c>
       <c r="E68">
         <v>0</v>
@@ -2967,7 +2934,7 @@
         <v>0</v>
       </c>
       <c r="H68">
-        <v>296</v>
+        <v>114</v>
       </c>
     </row>
     <row r="69" spans="1:8">
@@ -2975,13 +2942,13 @@
         <v>74</v>
       </c>
       <c r="B69">
-        <v>0.1485714285714286</v>
+        <v>0.1008064516129032</v>
       </c>
       <c r="C69">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D69">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="E69">
         <v>0</v>
@@ -2993,7 +2960,7 @@
         <v>0</v>
       </c>
       <c r="H69">
-        <v>149</v>
+        <v>223</v>
       </c>
     </row>
     <row r="70" spans="1:8">
@@ -3001,13 +2968,13 @@
         <v>75</v>
       </c>
       <c r="B70">
-        <v>0.1384615384615385</v>
+        <v>0.09863013698630137</v>
       </c>
       <c r="C70">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="D70">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="E70">
         <v>0</v>
@@ -3019,7 +2986,7 @@
         <v>0</v>
       </c>
       <c r="H70">
-        <v>112</v>
+        <v>329</v>
       </c>
     </row>
     <row r="71" spans="1:8">
@@ -3027,13 +2994,13 @@
         <v>76</v>
       </c>
       <c r="B71">
-        <v>0.1273885350318471</v>
+        <v>0.09836065573770492</v>
       </c>
       <c r="C71">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="D71">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="E71">
         <v>0</v>
@@ -3045,7 +3012,7 @@
         <v>0</v>
       </c>
       <c r="H71">
-        <v>137</v>
+        <v>165</v>
       </c>
     </row>
     <row r="72" spans="1:8">
@@ -3053,13 +3020,13 @@
         <v>77</v>
       </c>
       <c r="B72">
-        <v>0.1145374449339207</v>
+        <v>0.09740259740259741</v>
       </c>
       <c r="C72">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="D72">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="E72">
         <v>0</v>
@@ -3071,7 +3038,7 @@
         <v>0</v>
       </c>
       <c r="H72">
-        <v>402</v>
+        <v>139</v>
       </c>
     </row>
     <row r="73" spans="1:8">
@@ -3079,13 +3046,13 @@
         <v>78</v>
       </c>
       <c r="B73">
-        <v>0.1129032258064516</v>
+        <v>0.08900523560209424</v>
       </c>
       <c r="C73">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="D73">
-        <v>28</v>
+        <v>17</v>
       </c>
       <c r="E73">
         <v>0</v>
@@ -3097,7 +3064,7 @@
         <v>0</v>
       </c>
       <c r="H73">
-        <v>220</v>
+        <v>174</v>
       </c>
     </row>
     <row r="74" spans="1:8">
@@ -3105,13 +3072,13 @@
         <v>79</v>
       </c>
       <c r="B74">
-        <v>0.1013698630136986</v>
+        <v>0.08333333333333333</v>
       </c>
       <c r="C74">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="D74">
-        <v>37</v>
+        <v>16</v>
       </c>
       <c r="E74">
         <v>0</v>
@@ -3123,7 +3090,7 @@
         <v>0</v>
       </c>
       <c r="H74">
-        <v>328</v>
+        <v>176</v>
       </c>
     </row>
     <row r="75" spans="1:8">
@@ -3131,13 +3098,13 @@
         <v>80</v>
       </c>
       <c r="B75">
-        <v>0.08743169398907104</v>
+        <v>0.08239700374531835</v>
       </c>
       <c r="C75">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="D75">
-        <v>16</v>
+        <v>22</v>
       </c>
       <c r="E75">
         <v>0</v>
@@ -3149,7 +3116,7 @@
         <v>0</v>
       </c>
       <c r="H75">
-        <v>167</v>
+        <v>245</v>
       </c>
     </row>
     <row r="76" spans="1:8">
@@ -3157,25 +3124,25 @@
         <v>81</v>
       </c>
       <c r="B76">
-        <v>0.08614232209737828</v>
+        <v>0.0797872340425532</v>
       </c>
       <c r="C76">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D76">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="E76">
-        <v>0</v>
+        <v>0.06</v>
       </c>
       <c r="F76">
-        <v>1</v>
+        <v>0.9399999999999999</v>
       </c>
       <c r="G76" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H76">
-        <v>244</v>
+        <v>173</v>
       </c>
     </row>
     <row r="77" spans="1:8">
@@ -3183,13 +3150,13 @@
         <v>82</v>
       </c>
       <c r="B77">
-        <v>0.08333333333333333</v>
+        <v>0.06760563380281689</v>
       </c>
       <c r="C77">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="D77">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="E77">
         <v>0</v>
@@ -3201,7 +3168,7 @@
         <v>0</v>
       </c>
       <c r="H77">
-        <v>176</v>
+        <v>331</v>
       </c>
     </row>
     <row r="78" spans="1:8">
@@ -3209,25 +3176,25 @@
         <v>83</v>
       </c>
       <c r="B78">
-        <v>0.08214285714285714</v>
+        <v>0.06589785831960461</v>
       </c>
       <c r="C78">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="D78">
-        <v>23</v>
+        <v>41</v>
       </c>
       <c r="E78">
-        <v>0</v>
+        <v>0.02</v>
       </c>
       <c r="F78">
-        <v>1</v>
+        <v>0.98</v>
       </c>
       <c r="G78" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H78">
-        <v>257</v>
+        <v>567</v>
       </c>
     </row>
     <row r="79" spans="1:8">
@@ -3235,25 +3202,25 @@
         <v>84</v>
       </c>
       <c r="B79">
-        <v>0.07755775577557755</v>
+        <v>0.06071428571428571</v>
       </c>
       <c r="C79">
-        <v>47</v>
+        <v>17</v>
       </c>
       <c r="D79">
-        <v>49</v>
+        <v>17</v>
       </c>
       <c r="E79">
-        <v>0.04</v>
+        <v>0</v>
       </c>
       <c r="F79">
-        <v>0.96</v>
+        <v>1</v>
       </c>
       <c r="G79" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H79">
-        <v>559</v>
+        <v>263</v>
       </c>
     </row>
     <row r="80" spans="1:8">
@@ -3261,13 +3228,13 @@
         <v>85</v>
       </c>
       <c r="B80">
-        <v>0.0645879732739421</v>
+        <v>0.05122494432071269</v>
       </c>
       <c r="C80">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="D80">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="E80">
         <v>0</v>
@@ -3279,7 +3246,7 @@
         <v>0</v>
       </c>
       <c r="H80">
-        <v>420</v>
+        <v>426</v>
       </c>
     </row>
     <row r="81" spans="1:8">
@@ -3287,25 +3254,25 @@
         <v>86</v>
       </c>
       <c r="B81">
-        <v>0.05379746835443038</v>
+        <v>0.04640371229698376</v>
       </c>
       <c r="C81">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="D81">
-        <v>18</v>
+        <v>23</v>
       </c>
       <c r="E81">
-        <v>0.06</v>
+        <v>0.13</v>
       </c>
       <c r="F81">
-        <v>0.9399999999999999</v>
+        <v>0.87</v>
       </c>
       <c r="G81" t="b">
         <v>1</v>
       </c>
       <c r="H81">
-        <v>299</v>
+        <v>411</v>
       </c>
     </row>
     <row r="82" spans="1:8">
@@ -3313,25 +3280,25 @@
         <v>87</v>
       </c>
       <c r="B82">
-        <v>0.04788732394366197</v>
+        <v>0.03539823008849557</v>
       </c>
       <c r="C82">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="D82">
-        <v>17</v>
+        <v>31</v>
       </c>
       <c r="E82">
-        <v>0</v>
+        <v>0.1</v>
       </c>
       <c r="F82">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="G82" t="b">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H82">
-        <v>338</v>
+        <v>763</v>
       </c>
     </row>
     <row r="83" spans="1:8">
@@ -3339,13 +3306,13 @@
         <v>88</v>
       </c>
       <c r="B83">
-        <v>0.04672897196261682</v>
+        <v>0.0290519877675841</v>
       </c>
       <c r="C83">
+        <v>19</v>
+      </c>
+      <c r="D83">
         <v>20</v>
-      </c>
-      <c r="D83">
-        <v>21</v>
       </c>
       <c r="E83">
         <v>0.05</v>
@@ -3357,59 +3324,7 @@
         <v>1</v>
       </c>
       <c r="H83">
-        <v>408</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8">
-      <c r="A84" s="1" t="s">
-        <v>89</v>
-      </c>
-      <c r="B84">
-        <v>0.02784810126582278</v>
-      </c>
-      <c r="C84">
-        <v>22</v>
-      </c>
-      <c r="D84">
-        <v>26</v>
-      </c>
-      <c r="E84">
-        <v>0.15</v>
-      </c>
-      <c r="F84">
-        <v>0.85</v>
-      </c>
-      <c r="G84" t="b">
-        <v>1</v>
-      </c>
-      <c r="H84">
-        <v>768</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8">
-      <c r="A85" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B85">
-        <v>0.02599388379204893</v>
-      </c>
-      <c r="C85">
-        <v>17</v>
-      </c>
-      <c r="D85">
-        <v>18</v>
-      </c>
-      <c r="E85">
-        <v>0.06</v>
-      </c>
-      <c r="F85">
-        <v>0.9399999999999999</v>
-      </c>
-      <c r="G85" t="b">
-        <v>1</v>
-      </c>
-      <c r="H85">
-        <v>637</v>
+        <v>635</v>
       </c>
     </row>
   </sheetData>

</xml_diff>